<commit_message>
rename code files and upload documents
</commit_message>
<xml_diff>
--- a/document/HomeCredit_feature_정리.xlsx
+++ b/document/HomeCredit_feature_정리.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\machine_learning\kaggle\home_credit_default_risk\home-credit-default-risk\document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9690"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="HomeCredit_columns_description" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HomeCredit_columns_description!$A$1:$H$219</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -2165,7 +2170,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3162,7 +3167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3170,10 +3175,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F23" sqref="C23:F23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3210,7 +3216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3233,7 +3239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3279,7 +3285,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3302,7 +3308,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3348,7 +3354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3371,7 +3377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3394,7 +3400,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3417,7 +3423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3440,7 +3446,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3463,7 +3469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3509,7 +3515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3532,7 +3538,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3630,7 +3636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3656,7 +3662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3682,7 +3688,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3708,7 +3714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3731,7 +3737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3754,7 +3760,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3777,7 +3783,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3800,7 +3806,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3823,7 +3829,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -3846,7 +3852,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3869,7 +3875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -3915,7 +3921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3938,7 +3944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3961,7 +3967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3984,7 +3990,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -4010,7 +4016,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -4033,7 +4039,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -4056,7 +4062,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -4079,7 +4085,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -4102,7 +4108,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -4125,7 +4131,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -4148,7 +4154,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -4171,7 +4177,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -4197,7 +4203,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -4223,7 +4229,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -4275,7 +4281,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -4301,7 +4307,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -4327,7 +4333,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -4353,7 +4359,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -4379,7 +4385,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -4405,7 +4411,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -4457,7 +4463,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -4509,7 +4515,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -4535,7 +4541,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -4561,7 +4567,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -4587,7 +4593,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -4639,7 +4645,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -4665,7 +4671,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -4691,7 +4697,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -4717,7 +4723,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -4743,7 +4749,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -4769,7 +4775,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -4795,7 +4801,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -4821,7 +4827,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -4847,7 +4853,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -4873,7 +4879,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -4899,7 +4905,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -4925,7 +4931,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -4951,7 +4957,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -4977,7 +4983,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -5003,7 +5009,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -5029,7 +5035,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -5081,7 +5087,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -5107,7 +5113,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -5133,7 +5139,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -5159,7 +5165,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -5185,7 +5191,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -5211,7 +5217,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -5237,7 +5243,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -5263,7 +5269,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -5289,7 +5295,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -5315,7 +5321,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -5341,7 +5347,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -5367,7 +5373,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -5393,7 +5399,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -5419,7 +5425,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -5445,7 +5451,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -5471,7 +5477,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -5494,7 +5500,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -5517,7 +5523,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -5540,7 +5546,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -5563,7 +5569,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -5586,7 +5592,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -5609,7 +5615,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -5632,7 +5638,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -5655,7 +5661,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -5678,7 +5684,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -5701,7 +5707,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -5724,7 +5730,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -5747,7 +5753,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -5770,7 +5776,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -5793,7 +5799,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -5816,7 +5822,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -5839,7 +5845,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -5862,7 +5868,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -5885,7 +5891,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -5908,7 +5914,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -5931,7 +5937,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -5954,7 +5960,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -5977,7 +5983,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -6000,7 +6006,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -6023,7 +6029,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -6046,7 +6052,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -6069,7 +6075,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -6092,7 +6098,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -6115,7 +6121,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -6138,7 +6144,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -6161,7 +6167,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -6184,7 +6190,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -6210,7 +6216,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -6236,7 +6242,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -6259,7 +6265,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -6282,7 +6288,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -6305,7 +6311,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -6328,7 +6334,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -6351,7 +6357,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -6374,7 +6380,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -6397,7 +6403,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -6423,7 +6429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -6446,7 +6452,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -6469,7 +6475,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -6492,7 +6498,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -6518,7 +6524,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -6544,7 +6550,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -6570,7 +6576,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -6593,7 +6599,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="141" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="5">
         <v>140</v>
       </c>
@@ -6616,7 +6622,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -6642,7 +6648,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -6665,7 +6671,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="5">
         <v>143</v>
       </c>
@@ -6688,7 +6694,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -6711,7 +6717,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -6734,7 +6740,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -6757,7 +6763,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -6780,7 +6786,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -6803,7 +6809,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -6826,7 +6832,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -6847,7 +6853,7 @@
       </c>
       <c r="G151" s="4"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -6868,7 +6874,7 @@
       </c>
       <c r="G152" s="4"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -6889,7 +6895,7 @@
       </c>
       <c r="G153" s="4"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -6910,7 +6916,7 @@
       </c>
       <c r="G154" s="4"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -6931,7 +6937,7 @@
       </c>
       <c r="G155" s="4"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -6952,7 +6958,7 @@
       </c>
       <c r="G156" s="4"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -6973,7 +6979,7 @@
       </c>
       <c r="G157" s="4"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -6994,7 +7000,7 @@
       </c>
       <c r="G158" s="4"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -7015,7 +7021,7 @@
       </c>
       <c r="G159" s="4"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -7036,7 +7042,7 @@
       </c>
       <c r="G160" s="4"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -7057,7 +7063,7 @@
       </c>
       <c r="G161" s="4"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -7083,7 +7089,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -7109,7 +7115,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -7132,7 +7138,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -7158,7 +7164,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -7184,7 +7190,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -7207,7 +7213,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -7233,7 +7239,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -7259,7 +7265,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -7282,7 +7288,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -7305,7 +7311,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -7328,7 +7334,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="4">
         <v>172</v>
       </c>
@@ -7351,7 +7357,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -7374,7 +7380,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -7397,7 +7403,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -7420,7 +7426,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -7446,7 +7452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -7469,7 +7475,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" s="4">
         <v>178</v>
       </c>
@@ -7495,7 +7501,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" s="4">
         <v>179</v>
       </c>
@@ -7521,7 +7527,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="4">
         <v>180</v>
       </c>
@@ -8440,7 +8446,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H219"/>
+  <autoFilter ref="A1:H219">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="credit_card_balance.csv"/>
+        <filter val="installments_payments.csv"/>
+        <filter val="POS_CASH_balance.csv"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>